<commit_message>
Atualizações script e planilha
</commit_message>
<xml_diff>
--- a/AS01/Sistema/Planilha dados fictícios.xlsx
+++ b/AS01/Sistema/Planilha dados fictícios.xlsx
@@ -12,42 +12,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="201">
+  <si>
+    <t>Nome</t>
+  </si>
   <si>
     <t>Marca</t>
   </si>
   <si>
-    <t>Nome</t>
-  </si>
-  <si>
     <t>Modelo</t>
   </si>
   <si>
     <t>CPF</t>
   </si>
   <si>
+    <t>Ano</t>
+  </si>
+  <si>
+    <t>Placa</t>
+  </si>
+  <si>
     <t>Sexo</t>
   </si>
   <si>
-    <t>Ano</t>
+    <t>Cor</t>
+  </si>
+  <si>
+    <t>Script</t>
   </si>
   <si>
     <t>dataNascimento</t>
   </si>
   <si>
-    <t>Placa</t>
-  </si>
-  <si>
     <t>RG</t>
   </si>
   <si>
-    <t>Cor</t>
-  </si>
-  <si>
     <t>Nacionalidade</t>
   </si>
   <si>
-    <t>Script</t>
+    <t>Buggy</t>
   </si>
   <si>
     <t>Telefone</t>
@@ -56,9 +59,6 @@
     <t>Lucas Jorge Souza</t>
   </si>
   <si>
-    <t>Buggy</t>
-  </si>
-  <si>
     <t>Buggy 1.6 2-Lug.</t>
   </si>
   <si>
@@ -74,6 +74,9 @@
     <t>Bege</t>
   </si>
   <si>
+    <t>1997-04-08'</t>
+  </si>
+  <si>
     <t>26.079.729-7</t>
   </si>
   <si>
@@ -107,67 +110,109 @@
     <t>Verde</t>
   </si>
   <si>
+    <t>208 Griffe 1.6 Flex 16V 5p Aut.</t>
+  </si>
+  <si>
+    <t>MUB-1522</t>
+  </si>
+  <si>
+    <t>Amarelo</t>
+  </si>
+  <si>
+    <t>Chrysler</t>
+  </si>
+  <si>
+    <t>Caravan LX 3.3 V6 182cv</t>
+  </si>
+  <si>
+    <t>MXU-1386</t>
+  </si>
+  <si>
     <t>Cláudio Henrique Oliver Oliveira</t>
   </si>
   <si>
-    <t>208 Griffe 1.6 Flex 16V 5p Aut.</t>
-  </si>
-  <si>
     <t>830.326.193-27</t>
   </si>
   <si>
-    <t>MUB-1522</t>
+    <t>1968-11-05'</t>
   </si>
   <si>
     <t>28.530.352-1</t>
   </si>
   <si>
-    <t>Amarelo</t>
+    <t>Mercury</t>
   </si>
   <si>
     <t>(11) 2678-5503</t>
   </si>
   <si>
-    <t>Chrysler</t>
+    <t>Sable LS 3.0 V6</t>
+  </si>
+  <si>
+    <t>NAW-7999</t>
   </si>
   <si>
     <t>Marcos Cauê Almada</t>
   </si>
   <si>
-    <t>Caravan LX 3.3 V6 182cv</t>
-  </si>
-  <si>
     <t>800.205.859-34</t>
   </si>
   <si>
-    <t>MXU-1386</t>
+    <t>VW - VolksWagen</t>
+  </si>
+  <si>
+    <t>1974-08-26'</t>
   </si>
   <si>
     <t>14.466.194-9</t>
   </si>
   <si>
+    <t>Gol Special/ Special Xtreme 1.0 Mi 2p</t>
+  </si>
+  <si>
+    <t>ABG-8752</t>
+  </si>
+  <si>
     <t>(84) 2540-9362</t>
   </si>
   <si>
+    <t>Kia Motors</t>
+  </si>
+  <si>
+    <t>Sportage EX 2.0 16V Mec.</t>
+  </si>
+  <si>
     <t>Vinicius Caio Enrico da Luz</t>
   </si>
   <si>
     <t>010.428.016-65</t>
   </si>
   <si>
+    <t>NAX-7680</t>
+  </si>
+  <si>
+    <t>Prata</t>
+  </si>
+  <si>
+    <t>1991-01-03'</t>
+  </si>
+  <si>
     <t>36.310.070-2</t>
   </si>
   <si>
     <t>(84) 3824-9182</t>
   </si>
   <si>
-    <t>Mercury</t>
-  </si>
-  <si>
-    <t>Sable LS 3.0 V6</t>
-  </si>
-  <si>
-    <t>NAW-7999</t>
+    <t>Nissan</t>
+  </si>
+  <si>
+    <t>Frontier XE  CD 4x4 2.5 TB Diesel</t>
+  </si>
+  <si>
+    <t>KDU-6335</t>
+  </si>
+  <si>
+    <t>Preto</t>
   </si>
   <si>
     <t>Alexandre Renan Rocha</t>
@@ -176,55 +221,58 @@
     <t>110.994.805-07</t>
   </si>
   <si>
+    <t>1995-01-03'</t>
+  </si>
+  <si>
     <t>31.551.814-5</t>
   </si>
   <si>
+    <t>Audi</t>
+  </si>
+  <si>
     <t>(92) 3932-0284</t>
   </si>
   <si>
+    <t>Q3 1.4 TFSI 150cv S-tronic 5p</t>
+  </si>
+  <si>
+    <t>NDP-8929</t>
+  </si>
+  <si>
+    <t>Branco</t>
+  </si>
+  <si>
+    <t>80 S2 Avant</t>
+  </si>
+  <si>
     <t>Fábio Luan Peixoto</t>
   </si>
   <si>
+    <t>CED-9021</t>
+  </si>
+  <si>
     <t>794.425.833-28</t>
   </si>
   <si>
-    <t>VW - VolksWagen</t>
-  </si>
-  <si>
-    <t>Gol Special/ Special Xtreme 1.0 Mi 2p</t>
-  </si>
-  <si>
-    <t>ABG-8752</t>
-  </si>
-  <si>
-    <t>Kia Motors</t>
+    <t>Dourado</t>
+  </si>
+  <si>
+    <t>1995-11-12'</t>
   </si>
   <si>
     <t>11.149.389-4</t>
   </si>
   <si>
-    <t>Sportage EX 2.0 16V Mec.</t>
-  </si>
-  <si>
-    <t>NAX-7680</t>
-  </si>
-  <si>
     <t>(98) 3997-9282</t>
   </si>
   <si>
-    <t>Prata</t>
-  </si>
-  <si>
-    <t>Nissan</t>
-  </si>
-  <si>
-    <t>Frontier XE  CD 4x4 2.5 TB Diesel</t>
-  </si>
-  <si>
-    <t>KDU-6335</t>
-  </si>
-  <si>
-    <t>Preto</t>
+    <t>Citroen</t>
+  </si>
+  <si>
+    <t>C3 X-BOX ONE 1.6 VTi Flex 16V 5p Mec.</t>
+  </si>
+  <si>
+    <t>NAA-3067</t>
   </si>
   <si>
     <t>Matheus Yuri Silva</t>
@@ -233,22 +281,22 @@
     <t>902.418.980-21</t>
   </si>
   <si>
+    <t>1981-04-03'</t>
+  </si>
+  <si>
     <t>21.373.999-9</t>
   </si>
   <si>
+    <t>Asia Motors</t>
+  </si>
+  <si>
     <t>(95) 2661-6424</t>
   </si>
   <si>
-    <t>Audi</t>
-  </si>
-  <si>
-    <t>Q3 1.4 TFSI 150cv S-tronic 5p</t>
-  </si>
-  <si>
-    <t>NDP-8929</t>
-  </si>
-  <si>
-    <t>Branco</t>
+    <t>Towner Multiuso 5p</t>
+  </si>
+  <si>
+    <t>JSR-7086</t>
   </si>
   <si>
     <t>José Caio Barbosa</t>
@@ -257,52 +305,64 @@
     <t>293.482.312-19</t>
   </si>
   <si>
-    <t>80 S2 Avant</t>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>320iA 2.0 TB M Sport ActiveFlex 16V 4p</t>
+  </si>
+  <si>
+    <t>1988-08-17'</t>
+  </si>
+  <si>
+    <t>AER-3936</t>
   </si>
   <si>
     <t>50.585.236-6</t>
   </si>
   <si>
-    <t>CED-9021</t>
-  </si>
-  <si>
-    <t>Dourado</t>
-  </si>
-  <si>
     <t>(96) 2721-9132</t>
   </si>
   <si>
-    <t>Citroen</t>
+    <t>M3 Cabrio 3.0 24V</t>
+  </si>
+  <si>
+    <t>JKA-2822</t>
+  </si>
+  <si>
+    <t>Azul</t>
   </si>
   <si>
     <t>Isabela Isabelly Ayla Costa</t>
   </si>
   <si>
-    <t>C3 X-BOX ONE 1.6 VTi Flex 16V 5p Mec.</t>
-  </si>
-  <si>
     <t>442.006.520-64</t>
   </si>
   <si>
-    <t>NAA-3067</t>
-  </si>
-  <si>
     <t>F</t>
   </si>
   <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t>1988-04-03'</t>
+  </si>
+  <si>
+    <t>Civic Sedan LXL 1.7 16V 130cv Aut 4p</t>
+  </si>
+  <si>
     <t>48.746.532-5</t>
   </si>
   <si>
+    <t>IDF-1647</t>
+  </si>
+  <si>
     <t>(95) 2946-9632</t>
   </si>
   <si>
-    <t>Asia Motors</t>
-  </si>
-  <si>
-    <t>Towner Multiuso 5p</t>
-  </si>
-  <si>
-    <t>JSR-7086</t>
+    <t>Accord Sed</t>
+  </si>
+  <si>
+    <t>BDU-0516</t>
   </si>
   <si>
     <t>Thomas Caio Ian Fogaça</t>
@@ -311,16 +371,31 @@
     <t>305.513.564-48</t>
   </si>
   <si>
+    <t>1953-04-26'</t>
+  </si>
+  <si>
     <t>28.917.909-9</t>
   </si>
   <si>
+    <t>Hyundai</t>
+  </si>
+  <si>
+    <t>HB20 Premium 1.6 Flex 16V Aut.</t>
+  </si>
+  <si>
     <t>(81) 3709-4275</t>
   </si>
   <si>
-    <t>BMW</t>
-  </si>
-  <si>
-    <t>320iA 2.0 TB M Sport ActiveFlex 16V 4p</t>
+    <t>JNT-1726</t>
+  </si>
+  <si>
+    <t>Vermelho</t>
+  </si>
+  <si>
+    <t>H100 GS Diesel (12 lugares)</t>
+  </si>
+  <si>
+    <t>IPC-9026</t>
   </si>
   <si>
     <t>Milena Juliana Santos</t>
@@ -329,154 +404,121 @@
     <t>434.566.012-20</t>
   </si>
   <si>
-    <t>AER-3936</t>
+    <t>1962-09-26'</t>
   </si>
   <si>
     <t>47.647.321-4</t>
   </si>
   <si>
+    <t>456 GT</t>
+  </si>
+  <si>
+    <t>HRL-6492</t>
+  </si>
+  <si>
     <t>(96) 3875-4248</t>
   </si>
   <si>
+    <t>F458 Speciale F1 4.5 V8</t>
+  </si>
+  <si>
     <t>Nina Patrícia Sales</t>
   </si>
   <si>
+    <t>LVQ-2632</t>
+  </si>
+  <si>
+    <t>Marrom</t>
+  </si>
+  <si>
     <t>947.487.728-91</t>
   </si>
   <si>
+    <t>1975-08-11'</t>
+  </si>
+  <si>
     <t>10.944.688-4</t>
   </si>
   <si>
     <t>(31) 3957-4998</t>
   </si>
   <si>
-    <t>M3 Cabrio 3.0 24V</t>
+    <t>Fiat</t>
+  </si>
+  <si>
+    <t>LINEA 1.9/ HLX 1.9/1.8 Flex  Dualogic 4p</t>
+  </si>
+  <si>
+    <t>MHK-4596</t>
+  </si>
+  <si>
+    <t>Palio SPORTING Dualogic 1.6 Flex 16V 5p</t>
+  </si>
+  <si>
+    <t>HVL-9891</t>
+  </si>
+  <si>
+    <t>Ford</t>
+  </si>
+  <si>
+    <t>F-100 Super S</t>
+  </si>
+  <si>
+    <t>HXL-6361</t>
+  </si>
+  <si>
+    <t>Ranger XLS 3.2 20V 4x4 CD Diesel Mec.</t>
+  </si>
+  <si>
+    <t>KAA-2642</t>
   </si>
   <si>
     <t>Melissa Laís Ramos</t>
   </si>
   <si>
-    <t>JKA-2822</t>
-  </si>
-  <si>
     <t>901.793.448-46</t>
   </si>
   <si>
-    <t>Azul</t>
+    <t>1990-07-06'</t>
   </si>
   <si>
     <t>20.712.177-1</t>
   </si>
   <si>
+    <t>Jeep</t>
+  </si>
+  <si>
     <t>(92) 3933-7643</t>
   </si>
   <si>
+    <t>Wrangler SAHARA 3.8 V6 199cv 2p</t>
+  </si>
+  <si>
+    <t>HZT-5412</t>
+  </si>
+  <si>
+    <t>Jaguar</t>
+  </si>
+  <si>
+    <t>XE 2.0 Turbocharged R-Sport 240cv Aut.</t>
+  </si>
+  <si>
     <t>Renato Ryan Nascimento</t>
   </si>
   <si>
+    <t>FKO-5391</t>
+  </si>
+  <si>
     <t>213.102.256-56</t>
   </si>
   <si>
-    <t>Honda</t>
-  </si>
-  <si>
-    <t>Civic Sedan LXL 1.7 16V 130cv Aut 4p</t>
+    <t>1989-07-11'</t>
   </si>
   <si>
     <t>42.501.689-4</t>
   </si>
   <si>
     <t>(11) 2860-8735</t>
-  </si>
-  <si>
-    <t>IDF-1647</t>
-  </si>
-  <si>
-    <t>Accord Sed</t>
-  </si>
-  <si>
-    <t>BDU-0516</t>
-  </si>
-  <si>
-    <t>Hyundai</t>
-  </si>
-  <si>
-    <t>HB20 Premium 1.6 Flex 16V Aut.</t>
-  </si>
-  <si>
-    <t>JNT-1726</t>
-  </si>
-  <si>
-    <t>Vermelho</t>
-  </si>
-  <si>
-    <t>H100 GS Diesel (12 lugares)</t>
-  </si>
-  <si>
-    <t>IPC-9026</t>
-  </si>
-  <si>
-    <t>456 GT</t>
-  </si>
-  <si>
-    <t>HRL-6492</t>
-  </si>
-  <si>
-    <t>F458 Speciale F1 4.5 V8</t>
-  </si>
-  <si>
-    <t>LVQ-2632</t>
-  </si>
-  <si>
-    <t>Marrom</t>
-  </si>
-  <si>
-    <t>Fiat</t>
-  </si>
-  <si>
-    <t>LINEA 1.9/ HLX 1.9/1.8 Flex  Dualogic 4p</t>
-  </si>
-  <si>
-    <t>MHK-4596</t>
-  </si>
-  <si>
-    <t>Palio SPORTING Dualogic 1.6 Flex 16V 5p</t>
-  </si>
-  <si>
-    <t>HVL-9891</t>
-  </si>
-  <si>
-    <t>Ford</t>
-  </si>
-  <si>
-    <t>F-100 Super S</t>
-  </si>
-  <si>
-    <t>HXL-6361</t>
-  </si>
-  <si>
-    <t>Ranger XLS 3.2 20V 4x4 CD Diesel Mec.</t>
-  </si>
-  <si>
-    <t>KAA-2642</t>
-  </si>
-  <si>
-    <t>Jeep</t>
-  </si>
-  <si>
-    <t>Wrangler SAHARA 3.8 V6 199cv 2p</t>
-  </si>
-  <si>
-    <t>HZT-5412</t>
-  </si>
-  <si>
-    <t>Jaguar</t>
-  </si>
-  <si>
-    <t>XE 2.0 Turbocharged R-Sport 240cv Aut.</t>
-  </si>
-  <si>
-    <t>FKO-5391</t>
   </si>
   <si>
     <t>XKR-S Coup</t>
@@ -580,8 +622,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
-    <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="164" formatCode="yyyy&quot;-&quot;mm&quot;-&quot;dd&quot;'&quot;"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -619,7 +661,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -639,10 +681,14 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0"/>
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -680,33 +726,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>16</v>
@@ -714,376 +760,627 @@
       <c r="C2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="6">
-        <v>35656.0</v>
+      <c r="D2" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H2" s="2" t="str">
-        <f t="shared" ref="H2:H15" si="1">"INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"',"&amp;D2&amp;",'"&amp;E2&amp;"','"&amp;F2&amp;"','"&amp;G2&amp;"');"</f>
-        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Lucas Jorge Souza','771.837.082-84','M',35656,'26.079.729-7','Brasileira','(82) 3714-4841');</v>
+        <f t="shared" ref="H2:H15" si="1">"INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('"&amp;A2&amp;"','"&amp;B2&amp;"','"&amp;C2&amp;"','"&amp;D2&amp;",'"&amp;E2&amp;"','"&amp;F2&amp;"','"&amp;G2&amp;"');"</f>
+        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Lucas Jorge Souza','771.837.082-84','M','1997-04-08','26.079.729-7','Brasileira','(82) 3714-4841');</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="6">
-        <v>35575.0</v>
+      <c r="D3" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="H3" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Cláudio Henrique Oliver Oliveira','830.326.193-27','M',35575,'28.530.352-1','Brasileira','(11) 2678-5503');</v>
+        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Cláudio Henrique Oliver Oliveira','830.326.193-27','M','1968-11-05','28.530.352-1','Brasileira','(11) 2678-5503');</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="6">
-        <v>25147.0</v>
+      <c r="D4" s="6" t="s">
+        <v>49</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="H4" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Marcos Cauê Almada','800.205.859-34','M',25147,'14.466.194-9','Brasileira','(84) 2540-9362');</v>
+        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Marcos Cauê Almada','800.205.859-34','M','1974-08-26','14.466.194-9','Brasileira','(84) 2540-9362');</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="6">
-        <v>27267.0</v>
+      <c r="D5" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="H5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Vinicius Caio Enrico da Luz','010.428.016-65','M',27267,'36.310.070-2','Brasileira','(84) 3824-9182');</v>
+        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Vinicius Caio Enrico da Luz','010.428.016-65','M','1991-01-03','36.310.070-2','Brasileira','(84) 3824-9182');</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="6">
-        <v>33241.0</v>
+      <c r="D6" s="6" t="s">
+        <v>69</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="H6" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Alexandre Renan Rocha','110.994.805-07','M',33241,'31.551.814-5','Brasileira','(92) 3932-0284');</v>
+        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Alexandre Renan Rocha','110.994.805-07','M','1995-01-03','31.551.814-5','Brasileira','(92) 3932-0284');</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="7">
-        <v>35015.0</v>
+      <c r="D7" s="6" t="s">
+        <v>81</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>62</v>
+        <v>82</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="H7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Fábio Luan Peixoto','794.425.833-28','M',35015,'11.149.389-4','Brasileira','(98) 3997-9282');</v>
+        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Fábio Luan Peixoto','794.425.833-28','M','1995-11-12','11.149.389-4','Brasileira','(98) 3997-9282');</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="6">
-        <v>29679.0</v>
+      <c r="D8" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
       <c r="H8" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Matheus Yuri Silva','902.418.980-21','M',29679,'21.373.999-9','Brasileira','(95) 2661-6424');</v>
+        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Matheus Yuri Silva','902.418.980-21','M','1981-04-03','21.373.999-9','Brasileira','(95) 2661-6424');</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="6">
-        <v>32372.0</v>
+      <c r="D9" s="6" t="s">
+        <v>99</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="H9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('José Caio Barbosa','293.482.312-19','M',32372,'50.585.236-6','Brasileira','(96) 2721-9132');</v>
+        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('José Caio Barbosa','293.482.312-19','M','1988-08-17','50.585.236-6','Brasileira','(96) 2721-9132');</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="6">
-        <v>32236.0</v>
+        <v>108</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>110</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>93</v>
+        <v>114</v>
       </c>
       <c r="H10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Isabela Isabelly Ayla Costa','442.006.520-64','F',32236,'48.746.532-5','Brasileira','(95) 2946-9632');</v>
+        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Isabela Isabelly Ayla Costa','442.006.520-64','F','1988-04-03','48.746.532-5','Brasileira','(95) 2946-9632');</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>98</v>
+        <v>118</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="6">
-        <v>19475.0</v>
+      <c r="D11" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>100</v>
+        <v>123</v>
       </c>
       <c r="H11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Thomas Caio Ian Fogaça','305.513.564-48','M',19475,'28.917.909-9','Brasileira','(81) 3709-4275');</v>
+        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Thomas Caio Ian Fogaça','305.513.564-48','M','1953-04-26','28.917.909-9','Brasileira','(81) 3709-4275');</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>103</v>
+        <v>128</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="6">
-        <v>22915.0</v>
+        <v>108</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>130</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>106</v>
+        <v>131</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="H12" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Milena Juliana Santos','434.566.012-20','F',22915,'47.647.321-4','Brasileira','(96) 3875-4248');</v>
+        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Milena Juliana Santos','434.566.012-20','F','1962-09-26','47.647.321-4','Brasileira','(96) 3875-4248');</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D13" s="6">
-        <v>27617.0</v>
+      <c r="D13" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>111</v>
+        <v>142</v>
       </c>
       <c r="H13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Nina Patrícia Sales','947.487.728-91','F',27617,'10.944.688-4','Brasileira','(31) 3957-4998');</v>
+        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Nina Patrícia Sales','947.487.728-91','F','1975-08-11','10.944.688-4','Brasileira','(31) 3957-4998');</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>113</v>
+        <v>153</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" s="6">
-        <v>33060.0</v>
+        <v>108</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>155</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>117</v>
+        <v>156</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>118</v>
+        <v>158</v>
       </c>
       <c r="H14" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Melissa Laís Ramos','901.793.448-46','F',33060,'20.712.177-1','Brasileira','(92) 3933-7643');</v>
+        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Melissa Laís Ramos','901.793.448-46','F','1990-07-06','20.712.177-1','Brasileira','(92) 3933-7643');</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>119</v>
+        <v>163</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="6">
-        <v>32700.0</v>
+      <c r="D15" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>123</v>
+        <v>167</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>124</v>
+        <v>168</v>
       </c>
       <c r="H15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Renato Ryan Nascimento','213.102.256-56','M',32700,'42.501.689-4','Brasileira','(11) 2860-8735');</v>
-      </c>
+        <v>INSERT INTO CLIENTE(NOME, CPF, SEXO, DATANASCIMENTO, RG, NACIONALIDADE, TELEFONE) VALUES('Renato Ryan Nascimento','213.102.256-56','M','1989-07-11','42.501.689-4','Brasileira','(11) 2860-8735');</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17">
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18">
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19">
+      <c r="D19" s="8"/>
     </row>
     <row r="20">
       <c r="B20" s="2"/>
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21">
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22">
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23">
+      <c r="C23" s="9"/>
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24">
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25">
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26">
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27">
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28">
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29">
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30">
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31">
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32">
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33">
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34">
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35">
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36">
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37">
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38">
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39">
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40">
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41">
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42">
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43">
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44">
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45">
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46">
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47">
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48">
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49">
+      <c r="D49" s="8"/>
+    </row>
+    <row r="50">
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51">
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52">
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53">
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54">
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55">
+      <c r="D55" s="8"/>
+    </row>
+    <row r="56">
+      <c r="D56" s="8"/>
+    </row>
+    <row r="57">
+      <c r="D57" s="8"/>
+    </row>
+    <row r="58">
+      <c r="D58" s="8"/>
+    </row>
+    <row r="59">
+      <c r="D59" s="8"/>
+    </row>
+    <row r="60">
+      <c r="D60" s="8"/>
+    </row>
+    <row r="61">
+      <c r="D61" s="8"/>
+    </row>
+    <row r="62">
+      <c r="D62" s="8"/>
+    </row>
+    <row r="63">
+      <c r="D63" s="8"/>
+    </row>
+    <row r="64">
+      <c r="D64" s="8"/>
+    </row>
+    <row r="65">
+      <c r="D65" s="8"/>
+    </row>
+    <row r="66">
+      <c r="D66" s="8"/>
+    </row>
+    <row r="67">
+      <c r="D67" s="8"/>
+    </row>
+    <row r="68">
+      <c r="D68" s="8"/>
+    </row>
+    <row r="69">
+      <c r="D69" s="8"/>
+    </row>
+    <row r="70">
+      <c r="D70" s="8"/>
+    </row>
+    <row r="71">
+      <c r="D71" s="8"/>
+    </row>
+    <row r="72">
+      <c r="D72" s="8"/>
+    </row>
+    <row r="73">
+      <c r="D73" s="8"/>
+    </row>
+    <row r="74">
+      <c r="D74" s="8"/>
+    </row>
+    <row r="75">
+      <c r="D75" s="8"/>
+    </row>
+    <row r="76">
+      <c r="D76" s="8"/>
+    </row>
+    <row r="77">
+      <c r="D77" s="8"/>
+    </row>
+    <row r="78">
+      <c r="D78" s="8"/>
+    </row>
+    <row r="79">
+      <c r="D79" s="8"/>
+    </row>
+    <row r="80">
+      <c r="D80" s="8"/>
+    </row>
+    <row r="81">
+      <c r="D81" s="8"/>
+    </row>
+    <row r="82">
+      <c r="D82" s="8"/>
+    </row>
+    <row r="83">
+      <c r="D83" s="8"/>
+    </row>
+    <row r="84">
+      <c r="D84" s="8"/>
+    </row>
+    <row r="85">
+      <c r="D85" s="8"/>
+    </row>
+    <row r="86">
+      <c r="D86" s="8"/>
+    </row>
+    <row r="87">
+      <c r="D87" s="8"/>
+    </row>
+    <row r="88">
+      <c r="D88" s="8"/>
+    </row>
+    <row r="89">
+      <c r="D89" s="8"/>
+    </row>
+    <row r="90">
+      <c r="D90" s="8"/>
+    </row>
+    <row r="91">
+      <c r="D91" s="8"/>
+    </row>
+    <row r="92">
+      <c r="D92" s="8"/>
+    </row>
+    <row r="93">
+      <c r="D93" s="8"/>
+    </row>
+    <row r="94">
+      <c r="D94" s="8"/>
+    </row>
+    <row r="95">
+      <c r="D95" s="8"/>
+    </row>
+    <row r="96">
+      <c r="D96" s="8"/>
+    </row>
+    <row r="97">
+      <c r="D97" s="8"/>
+    </row>
+    <row r="98">
+      <c r="D98" s="8"/>
+    </row>
+    <row r="99">
+      <c r="D99" s="8"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -1107,27 +1404,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>15</v>
@@ -1148,19 +1445,19 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4">
         <v>1995.0</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="1"/>
@@ -1169,19 +1466,19 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4">
         <v>1995.0</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="1"/>
@@ -1190,7 +1487,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>32</v>
@@ -1199,10 +1496,10 @@
         <v>2013.0</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="1"/>
@@ -1211,19 +1508,19 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C6" s="4">
         <v>2005.0</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="1"/>
@@ -1232,16 +1529,16 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C7" s="4">
         <v>1992.0</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>19</v>
@@ -1253,19 +1550,19 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C8" s="4">
         <v>1998.0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="1"/>
@@ -1274,19 +1571,19 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C9" s="4">
         <v>2008.0</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="1"/>
@@ -1295,19 +1592,19 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="C10" s="4">
         <v>2009.0</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="1"/>
@@ -1316,19 +1613,19 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C11" s="4">
         <v>2016.0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="1"/>
@@ -1337,19 +1634,19 @@
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C12" s="4">
         <v>1994.0</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="1"/>
@@ -1358,19 +1655,19 @@
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C13" s="4">
         <v>2014.0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="1"/>
@@ -1379,19 +1676,19 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C14" s="4">
         <v>1997.0</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="1"/>
@@ -1400,19 +1697,19 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C15" s="4">
         <v>2015.0</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="1"/>
@@ -1421,19 +1718,19 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C16" s="4">
         <v>1994.0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="1"/>
@@ -1442,19 +1739,19 @@
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="C17" s="4">
         <v>2005.0</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="1"/>
@@ -1463,19 +1760,19 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="C18" s="4">
         <v>2008.0</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="1"/>
@@ -1484,19 +1781,19 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="C19" s="4">
         <v>2013.0</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="1"/>
@@ -1505,19 +1802,19 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C20" s="4">
         <v>1994.0</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="1"/>
@@ -1526,19 +1823,19 @@
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C21" s="4">
         <v>1993.0</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="1"/>
@@ -1547,10 +1844,10 @@
     </row>
     <row r="22">
       <c r="A22" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C22" s="4">
         <v>2013.0</v>
@@ -1568,19 +1865,19 @@
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C23" s="4">
         <v>2009.0</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="1"/>
@@ -1589,19 +1886,19 @@
     </row>
     <row r="24">
       <c r="A24" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="C24" s="4">
         <v>2012.0</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="1"/>
@@ -1610,19 +1907,19 @@
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C25" s="4">
         <v>1985.0</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="1"/>
@@ -1631,19 +1928,19 @@
     </row>
     <row r="26">
       <c r="A26" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C26" s="4">
         <v>2013.0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="1"/>
@@ -1652,16 +1949,16 @@
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="C27" s="4">
         <v>2011.0</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>19</v>
@@ -1673,16 +1970,16 @@
     </row>
     <row r="28">
       <c r="A28" s="2" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="C28" s="4">
         <v>2016.0</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>138</v>
@@ -1694,19 +1991,19 @@
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>155</v>
+        <v>169</v>
       </c>
       <c r="C29" s="4">
         <v>2014.0</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>156</v>
+        <v>170</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="1"/>
@@ -1715,16 +2012,16 @@
     </row>
     <row r="30">
       <c r="A30" s="2" t="s">
-        <v>157</v>
+        <v>171</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>158</v>
+        <v>172</v>
       </c>
       <c r="C30" s="4">
         <v>2016.0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>159</v>
+        <v>173</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>138</v>
@@ -1736,19 +2033,19 @@
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="C31" s="4">
         <v>2006.0</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>161</v>
+        <v>175</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="1"/>
@@ -1757,19 +2054,19 @@
     </row>
     <row r="32">
       <c r="A32" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>162</v>
+        <v>176</v>
       </c>
       <c r="C32" s="4">
         <v>2012.0</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>163</v>
+        <v>177</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="1"/>
@@ -1778,16 +2075,16 @@
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>165</v>
+        <v>179</v>
       </c>
       <c r="C33" s="4">
         <v>2006.0</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>19</v>
@@ -1799,19 +2096,19 @@
     </row>
     <row r="34">
       <c r="A34" s="2" t="s">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="C34" s="4">
         <v>2001.0</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>168</v>
+        <v>182</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>169</v>
+        <v>183</v>
       </c>
       <c r="F34" t="str">
         <f t="shared" si="1"/>
@@ -1820,19 +2117,19 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="C35" s="4">
         <v>2002.0</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F35" t="str">
         <f t="shared" si="1"/>
@@ -1841,19 +2138,19 @@
     </row>
     <row r="36">
       <c r="A36" s="2" t="s">
-        <v>170</v>
+        <v>184</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="C36" s="4">
         <v>2013.0</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="F36" t="str">
         <f t="shared" si="1"/>
@@ -1862,16 +2159,16 @@
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="C37" s="4">
         <v>2014.0</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>19</v>
@@ -1883,19 +2180,19 @@
     </row>
     <row r="38">
       <c r="A38" s="2" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>179</v>
+        <v>193</v>
       </c>
       <c r="C38" s="4">
         <v>2011.0</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F38" t="str">
         <f t="shared" si="1"/>
@@ -1904,19 +2201,19 @@
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="C39" s="4">
         <v>1991.0</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="F39" t="str">
         <f t="shared" si="1"/>
@@ -1925,19 +2222,19 @@
     </row>
     <row r="40">
       <c r="A40" s="2" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>185</v>
+        <v>199</v>
       </c>
       <c r="C40" s="4">
         <v>2015.0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>186</v>
+        <v>200</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F40" t="str">
         <f t="shared" si="1"/>

</xml_diff>